<commit_message>
Updated .xslx with charts
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="21100" yWindow="2620" windowWidth="17300" windowHeight="17600" tabRatio="500"/>
+    <workbookView xWindow="7960" yWindow="2620" windowWidth="30440" windowHeight="17600" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="12">
   <si>
     <t>Manual</t>
   </si>
@@ -69,10 +69,26 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -95,13 +111,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -112,6 +132,2619 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> improvement vs. Grid Size (diameter)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$U$9:$U$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$V$9:$V$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>29.57732771363821</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.9781481164572</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>52.62442166459395</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2003098144"/>
+        <c:axId val="-2002969088"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2003098144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2002969088"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2002969088"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2003098144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> improvement vs. Road Width (# lanes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$X$9:$X$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$Y$9:$Y$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>58.78816334463666</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>46.42556615027537</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29.39652293143154</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1996780544"/>
+        <c:axId val="-1996945776"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1996780544"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1996945776"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-1996945776"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1996780544"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Percent</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> improvement vs. Road Width (# lanes)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$AA$9:$AA$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>10.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$AB$9:$AB$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>59.66398956962514</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.663315397845</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>23.85259252721922</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-1968292800"/>
+        <c:axId val="-2071749984"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-1968292800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2071749984"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2071749984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-1968292800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>158750</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,10 +3010,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R29"/>
+  <dimension ref="A1:AC29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA17" sqref="AA17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -398,7 +3031,7 @@
     <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -454,7 +3087,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -502,7 +3135,7 @@
         <v>28.662519631189099</v>
       </c>
       <c r="P2">
-        <f>AVERAGE(M2:O2)</f>
+        <f t="shared" ref="P2:P28" si="0">AVERAGE(M2:O2)</f>
         <v>35.877306636586702</v>
       </c>
       <c r="Q2">
@@ -514,7 +3147,7 @@
         <v>53.033265436015867</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -537,7 +3170,7 @@
         <v>17.1419806875071</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H28" si="0">AVERAGE(E3:G3)</f>
+        <f t="shared" ref="H3:H28" si="1">AVERAGE(E3:G3)</f>
         <v>17.5146230881472</v>
       </c>
       <c r="I3" t="s">
@@ -562,19 +3195,28 @@
         <v>32.505372762620802</v>
       </c>
       <c r="P3">
-        <f>AVERAGE(M3:O3)</f>
+        <f t="shared" si="0"/>
         <v>31.823950803429568</v>
       </c>
       <c r="Q3">
-        <f t="shared" ref="Q3:Q28" si="1">P3-H3</f>
+        <f t="shared" ref="Q3:Q28" si="2">P3-H3</f>
         <v>14.309327715282368</v>
       </c>
       <c r="R3">
-        <f t="shared" ref="R3:R28" si="2">(P3-H3)/H3 * 100</f>
+        <f t="shared" ref="R3:R28" si="3">(P3-H3)/H3 * 100</f>
         <v>81.6993185823452</v>
       </c>
+      <c r="U3" t="s">
+        <v>2</v>
+      </c>
+      <c r="X3" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -597,7 +3239,7 @@
         <v>17.6312444918713</v>
       </c>
       <c r="H4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.116452186302499</v>
       </c>
       <c r="I4" t="s">
@@ -622,19 +3264,46 @@
         <v>21.622938098159899</v>
       </c>
       <c r="P4">
-        <f>AVERAGE(M4:O4)</f>
+        <f t="shared" si="0"/>
         <v>22.02494177876623</v>
       </c>
       <c r="Q4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.9084895924637308</v>
       </c>
       <c r="R4">
         <f>(P4-H4)/H4 * 100</f>
         <v>21.574255004624273</v>
       </c>
+      <c r="U4">
+        <v>3</v>
+      </c>
+      <c r="V4">
+        <v>4</v>
+      </c>
+      <c r="W4">
+        <v>5</v>
+      </c>
+      <c r="X4">
+        <v>1</v>
+      </c>
+      <c r="Y4">
+        <v>2</v>
+      </c>
+      <c r="Z4">
+        <v>3</v>
+      </c>
+      <c r="AA4">
+        <v>10</v>
+      </c>
+      <c r="AB4">
+        <v>20</v>
+      </c>
+      <c r="AC4">
+        <v>30</v>
+      </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -657,7 +3326,7 @@
         <v>23.092792999260698</v>
       </c>
       <c r="H5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>24.279452716612031</v>
       </c>
       <c r="I5" t="s">
@@ -682,19 +3351,19 @@
         <v>42.612987193937798</v>
       </c>
       <c r="P5">
-        <f>AVERAGE(M5:O5)</f>
+        <f t="shared" si="0"/>
         <v>34.512650660885697</v>
       </c>
       <c r="Q5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.233197944273666</v>
       </c>
       <c r="R5">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>42.147564295269717</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -717,7 +3386,7 @@
         <v>25.514228714211001</v>
       </c>
       <c r="H6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>23.841788164958064</v>
       </c>
       <c r="I6" t="s">
@@ -742,19 +3411,19 @@
         <v>30.451880242703901</v>
       </c>
       <c r="P6">
-        <f>AVERAGE(M6:O6)</f>
+        <f t="shared" si="0"/>
         <v>29.939182891150836</v>
       </c>
       <c r="Q6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.0973947261927712</v>
       </c>
       <c r="R6">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>25.574401903102789</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -777,7 +3446,7 @@
         <v>18.718839200053299</v>
       </c>
       <c r="H7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.078005571053996</v>
       </c>
       <c r="I7" t="s">
@@ -802,19 +3471,19 @@
         <v>25.6850099107664</v>
       </c>
       <c r="P7">
-        <f>AVERAGE(M7:O7)</f>
+        <f t="shared" si="0"/>
         <v>27.635175293300097</v>
       </c>
       <c r="Q7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.5571697222461012</v>
       </c>
       <c r="R7">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>31.109061529288763</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -837,7 +3506,7 @@
         <v>24.289690510739302</v>
       </c>
       <c r="H8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.851289493619671</v>
       </c>
       <c r="I8" t="s">
@@ -862,19 +3531,19 @@
         <v>31.407874984984701</v>
       </c>
       <c r="P8">
-        <f>AVERAGE(M8:O8)</f>
+        <f t="shared" si="0"/>
         <v>28.278838696134766</v>
       </c>
       <c r="Q8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1.4275492025150953</v>
       </c>
       <c r="R8">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.3165014769748975</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -897,7 +3566,7 @@
         <v>26.1410006580467</v>
       </c>
       <c r="H9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>26.579094165423069</v>
       </c>
       <c r="I9" t="s">
@@ -922,19 +3591,40 @@
         <v>33.023852571769901</v>
       </c>
       <c r="P9">
-        <f>AVERAGE(M9:O9)</f>
+        <f t="shared" si="0"/>
         <v>27.313648819304603</v>
       </c>
       <c r="Q9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.73455465388153485</v>
       </c>
       <c r="R9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.7636557111758995</v>
       </c>
+      <c r="U9">
+        <v>3</v>
+      </c>
+      <c r="V9">
+        <f>AVERAGE(R2:R10)</f>
+        <v>29.577327713638208</v>
+      </c>
+      <c r="X9">
+        <v>1</v>
+      </c>
+      <c r="Y9">
+        <f>AVERAGE(R2:R4,R11:R13,R20:R22)</f>
+        <v>58.788163344636665</v>
+      </c>
+      <c r="AA9">
+        <v>10</v>
+      </c>
+      <c r="AB9">
+        <f>AVERAGE(R2,R5,R8,R11,R14,R17,R20,R23,R26)</f>
+        <v>59.663989569625137</v>
+      </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -957,7 +3647,7 @@
         <v>27.106472778377199</v>
       </c>
       <c r="H10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>25.774858814958431</v>
       </c>
       <c r="I10" t="s">
@@ -982,19 +3672,40 @@
         <v>21.857772621974298</v>
       </c>
       <c r="P10">
-        <f>AVERAGE(M10:O10)</f>
+        <f t="shared" si="0"/>
         <v>26.542414904060298</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.76755608910186623</v>
       </c>
       <c r="R10">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.9779254839464544</v>
       </c>
+      <c r="U10">
+        <v>4</v>
+      </c>
+      <c r="V10">
+        <f>AVERAGE(R11:R19)</f>
+        <v>44.978148116457206</v>
+      </c>
+      <c r="X10">
+        <v>2</v>
+      </c>
+      <c r="Y10">
+        <f>AVERAGE(R5:R7,R14:R16,R20:R22)</f>
+        <v>46.425566150275365</v>
+      </c>
+      <c r="AA10">
+        <v>20</v>
+      </c>
+      <c r="AB10">
+        <f>AVERAGE(R3,R6,R9,R12,R15,R18,R21,R24,R27)</f>
+        <v>43.663315397844997</v>
+      </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +3728,7 @@
         <v>21.023418903076401</v>
       </c>
       <c r="H11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.355388647415069</v>
       </c>
       <c r="I11" t="s">
@@ -1042,19 +3753,40 @@
         <v>30.023590640178099</v>
       </c>
       <c r="P11">
-        <f>AVERAGE(M11:O11)</f>
+        <f t="shared" si="0"/>
         <v>31.702736828182534</v>
       </c>
       <c r="Q11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.347348180767465</v>
       </c>
       <c r="R11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>63.792819693219982</v>
       </c>
+      <c r="U11">
+        <v>5</v>
+      </c>
+      <c r="V11">
+        <f>AVERAGE(R20:R28)</f>
+        <v>52.624421664593953</v>
+      </c>
+      <c r="X11">
+        <v>3</v>
+      </c>
+      <c r="Y11">
+        <f>AVERAGE(R8:R10,R17:R19,R26:R28)</f>
+        <v>29.396522931431541</v>
+      </c>
+      <c r="AA11">
+        <v>30</v>
+      </c>
+      <c r="AB11">
+        <f>AVERAGE(R4,R7,R10,R13,R16,R19,R22,R25,R28)</f>
+        <v>23.852592527219219</v>
+      </c>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1077,7 +3809,7 @@
         <v>13.854862113857401</v>
       </c>
       <c r="H12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.933844525134401</v>
       </c>
       <c r="I12" t="s">
@@ -1102,19 +3834,19 @@
         <v>27.991763732608799</v>
       </c>
       <c r="P12">
-        <f>AVERAGE(M12:O12)</f>
+        <f t="shared" si="0"/>
         <v>31.498330365019502</v>
       </c>
       <c r="Q12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.564485839885101</v>
       </c>
       <c r="R12">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>75.636240856634984</v>
       </c>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1137,7 +3869,7 @@
         <v>17.0247080240492</v>
       </c>
       <c r="H13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>16.804841245325136</v>
       </c>
       <c r="I13" t="s">
@@ -1162,19 +3894,19 @@
         <v>23.852694489703602</v>
       </c>
       <c r="P13">
-        <f>AVERAGE(M13:O13)</f>
+        <f t="shared" si="0"/>
         <v>23.104555095460398</v>
       </c>
       <c r="Q13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.2997138501352623</v>
       </c>
       <c r="R13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>37.487493979675364</v>
       </c>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +3929,7 @@
         <v>20.4521584280029</v>
       </c>
       <c r="H14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.126933890242899</v>
       </c>
       <c r="I14" t="s">
@@ -1222,19 +3954,19 @@
         <v>40.055632009757701</v>
       </c>
       <c r="P14">
-        <f>AVERAGE(M14:O14)</f>
+        <f t="shared" si="0"/>
         <v>33.864569746846236</v>
       </c>
       <c r="Q14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.737635856603337</v>
       </c>
       <c r="R14">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60.290981752378123</v>
       </c>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1257,7 +3989,7 @@
         <v>22.4345573241559</v>
       </c>
       <c r="H15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.719740802802864</v>
       </c>
       <c r="I15" t="s">
@@ -1282,19 +4014,19 @@
         <v>29.645712104533001</v>
       </c>
       <c r="P15">
-        <f>AVERAGE(M15:O15)</f>
+        <f t="shared" si="0"/>
         <v>29.039807482906635</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.3200666801037713</v>
       </c>
       <c r="R15">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>40.155264292583595</v>
       </c>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1317,7 +4049,7 @@
         <v>23.652963331993099</v>
       </c>
       <c r="H16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.93774277968663</v>
       </c>
       <c r="I16" t="s">
@@ -1342,15 +4074,15 @@
         <v>28.2520874891879</v>
       </c>
       <c r="P16">
-        <f>AVERAGE(M16:O16)</f>
+        <f t="shared" si="0"/>
         <v>26.913825039880802</v>
       </c>
       <c r="Q16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.9760822601941719</v>
       </c>
       <c r="R16">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>22.682745030640991</v>
       </c>
     </row>
@@ -1377,7 +4109,7 @@
         <v>20.555617225363999</v>
       </c>
       <c r="H17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.376570353734532</v>
       </c>
       <c r="I17" t="s">
@@ -1402,15 +4134,15 @@
         <v>40.059307924705102</v>
       </c>
       <c r="P17">
-        <f>AVERAGE(M17:O17)</f>
+        <f t="shared" si="0"/>
         <v>35.405230350582336</v>
       </c>
       <c r="Q17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.028659996847804</v>
       </c>
       <c r="R17">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>58.22456163249069</v>
       </c>
     </row>
@@ -1437,7 +4169,7 @@
         <v>23.1472923157609</v>
       </c>
       <c r="H18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.113521327557436</v>
       </c>
       <c r="I18" t="s">
@@ -1462,15 +4194,15 @@
         <v>28.702553623981998</v>
       </c>
       <c r="P18">
-        <f>AVERAGE(M18:O18)</f>
+        <f t="shared" si="0"/>
         <v>28.820525836586935</v>
       </c>
       <c r="Q18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.707004509029499</v>
       </c>
       <c r="R18">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>30.329880120319697</v>
       </c>
     </row>
@@ -1497,7 +4229,7 @@
         <v>20.728707301334801</v>
       </c>
       <c r="H19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.906302210662137</v>
       </c>
       <c r="I19" t="s">
@@ -1522,15 +4254,15 @@
         <v>25.5573748824695</v>
       </c>
       <c r="P19">
-        <f>AVERAGE(M19:O19)</f>
+        <f t="shared" si="0"/>
         <v>26.617889542691099</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.7115873320289623</v>
       </c>
       <c r="R19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16.20334569017141</v>
       </c>
     </row>
@@ -1557,7 +4289,7 @@
         <v>20.312143371427702</v>
       </c>
       <c r="H20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.483801082209165</v>
       </c>
       <c r="I20" t="s">
@@ -1582,15 +4314,15 @@
         <v>31.469759831784799</v>
       </c>
       <c r="P20">
-        <f>AVERAGE(M20:O20)</f>
+        <f t="shared" si="0"/>
         <v>38.281345777370639</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>18.797544695161474</v>
       </c>
       <c r="R20">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96.477810545528925</v>
       </c>
     </row>
@@ -1617,7 +4349,7 @@
         <v>17.6385493457562</v>
       </c>
       <c r="H21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>18.8465140623174</v>
       </c>
       <c r="I21" t="s">
@@ -1642,15 +4374,15 @@
         <v>27.955018835518999</v>
       </c>
       <c r="P21">
-        <f>AVERAGE(M21:O21)</f>
+        <f t="shared" si="0"/>
         <v>29.7676540979549</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>10.921140035637499</v>
       </c>
       <c r="R21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>57.947798725673813</v>
       </c>
     </row>
@@ -1677,7 +4409,7 @@
         <v>16.365042356704802</v>
       </c>
       <c r="H22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>17.140374611807999</v>
       </c>
       <c r="I22" t="s">
@@ -1702,15 +4434,15 @@
         <v>22.162716250813599</v>
       </c>
       <c r="P22">
-        <f>AVERAGE(M22:O22)</f>
+        <f t="shared" si="0"/>
         <v>24.244111559127365</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1037369473193657</v>
       </c>
       <c r="R22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>41.444467278011551</v>
       </c>
     </row>
@@ -1737,7 +4469,7 @@
         <v>22.691964705416002</v>
       </c>
       <c r="H23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>22.562696222396298</v>
       </c>
       <c r="I23" t="s">
@@ -1762,15 +4494,15 @@
         <v>39.137898101189101</v>
       </c>
       <c r="P23">
-        <f>AVERAGE(M23:O23)</f>
+        <f t="shared" si="0"/>
         <v>35.079769478770736</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>12.517073256374438</v>
       </c>
       <c r="R23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>55.476850519086796</v>
       </c>
     </row>
@@ -1797,7 +4529,7 @@
         <v>18.249023021107</v>
       </c>
       <c r="H24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>19.122652758430633</v>
       </c>
       <c r="I24" t="s">
@@ -1822,15 +4554,15 @@
         <v>25.1144448393947</v>
       </c>
       <c r="P24">
-        <f>AVERAGE(M24:O24)</f>
+        <f t="shared" si="0"/>
         <v>28.583498182450768</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.4608454240201354</v>
       </c>
       <c r="R24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>49.474544894662266</v>
       </c>
     </row>
@@ -1857,7 +4589,7 @@
         <v>20.205194927230998</v>
       </c>
       <c r="H25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.366906209765897</v>
       </c>
       <c r="I25" t="s">
@@ -1882,15 +4614,15 @@
         <v>25.92291896659</v>
       </c>
       <c r="P25">
-        <f>AVERAGE(M25:O25)</f>
+        <f t="shared" si="0"/>
         <v>25.264227943937669</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>4.8973217341717721</v>
       </c>
       <c r="R25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>24.045486750577339</v>
       </c>
     </row>
@@ -1917,7 +4649,7 @@
         <v>20.8241754290807</v>
       </c>
       <c r="H26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.704277815267265</v>
       </c>
       <c r="I26" t="s">
@@ -1942,15 +4674,15 @@
         <v>46.042439380790597</v>
       </c>
       <c r="P26">
-        <f>AVERAGE(M26:O26)</f>
+        <f t="shared" si="0"/>
         <v>43.889424926022365</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>22.1851471107551</v>
       </c>
       <c r="R26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>102.21555077566128</v>
       </c>
     </row>
@@ -1977,7 +4709,7 @@
         <v>20.2999476706051</v>
       </c>
       <c r="H27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>20.517779792152901</v>
       </c>
       <c r="I27" t="s">
@@ -2002,15 +4734,15 @@
         <v>26.915255988992801</v>
       </c>
       <c r="P27">
-        <f>AVERAGE(M27:O27)</f>
+        <f t="shared" si="0"/>
         <v>26.547695414176403</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.029915622023502</v>
       </c>
       <c r="R27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>29.388733494106734</v>
       </c>
     </row>
@@ -2037,7 +4769,7 @@
         <v>21.2180482425713</v>
       </c>
       <c r="H28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>21.049549320222734</v>
       </c>
       <c r="I28" t="s">
@@ -2062,15 +4794,15 @@
         <v>25.677371196681801</v>
       </c>
       <c r="P28">
-        <f>AVERAGE(M28:O28)</f>
+        <f t="shared" si="0"/>
         <v>24.659242230753534</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6096929105308</v>
       </c>
       <c r="R28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17.148551998036812</v>
       </c>
     </row>
@@ -2086,5 +4818,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added 2 more averages to the sheet
</commit_message>
<xml_diff>
--- a/test_results.xlsx
+++ b/test_results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobgold/PycharmProjects/Traffic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jacobgold/proj/Traffic/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="12">
   <si>
     <t>Manual</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>%Improvement</t>
-  </si>
-  <si>
-    <t>Averages:</t>
   </si>
 </sst>
 </file>
@@ -185,7 +182,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -282,11 +278,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2019324224"/>
-        <c:axId val="-1998850832"/>
+        <c:axId val="-2111180864"/>
+        <c:axId val="-2066296016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2019324224"/>
+        <c:axId val="-2111180864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -328,7 +324,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1998850832"/>
+        <c:crossAx val="-2066296016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -336,7 +332,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1998850832"/>
+        <c:axId val="-2066296016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -387,7 +383,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2019324224"/>
+        <c:crossAx val="-2111180864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -476,7 +472,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -573,11 +568,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2002970384"/>
-        <c:axId val="-2004625408"/>
+        <c:axId val="-2093047520"/>
+        <c:axId val="-2092455840"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2002970384"/>
+        <c:axId val="-2093047520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -620,7 +615,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2004625408"/>
+        <c:crossAx val="-2092455840"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -628,7 +623,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2004625408"/>
+        <c:axId val="-2092455840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -648,6 +643,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -678,7 +674,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2002970384"/>
+        <c:crossAx val="-2093047520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -767,7 +763,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -864,11 +859,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-1997487200"/>
-        <c:axId val="-1997293776"/>
+        <c:axId val="-2093933200"/>
+        <c:axId val="-2093846752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-1997487200"/>
+        <c:axId val="-2093933200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -910,7 +905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1997293776"/>
+        <c:crossAx val="-2093846752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -918,7 +913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1997293776"/>
+        <c:axId val="-2093846752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,7 +964,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1997487200"/>
+        <c:crossAx val="-2093933200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3021,8 +3016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="T38" sqref="T38"/>
+    <sheetView tabSelected="1" topLeftCell="C2" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4789,8 +4784,13 @@
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="P29" t="s">
-        <v>12</v>
+      <c r="H29">
+        <f>AVERAGE(H2:H28)</f>
+        <v>21.242560171628682</v>
+      </c>
+      <c r="P29">
+        <f>AVERAGE(P2:P28)</f>
+        <v>29.897501866012576</v>
       </c>
       <c r="Q29">
         <f>AVERAGE(Q2:Q28)</f>

</xml_diff>